<commit_message>
adding changes related to RemoteWebdriver
</commit_message>
<xml_diff>
--- a/testdata/Data.xlsx
+++ b/testdata/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swati/Desktop/BreakOutSessionDec2024/AugFramework/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8D4871-7BC0-2441-AA4F-9EB21D7C20B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D66075AB-D7F1-5248-88BC-668B700E94D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="new_users" sheetId="5" r:id="rId1"/>
@@ -79,7 +79,7 @@
     <t>Cypress</t>
   </si>
   <si>
-    <t>ora20@gmail.com</t>
+    <t>Himanshu_123@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>